<commit_message>
fixed bug with creating ReportRb excel
</commit_message>
<xml_diff>
--- a/files/reports/rb/rb_report_template.xlsx
+++ b/files/reports/rb/rb_report_template.xlsx
@@ -11,7 +11,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="305" uniqueCount="304">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="307" uniqueCount="306">
   <si>
     <t>Номенклатура</t>
   </si>
@@ -923,6 +923,12 @@
   </si>
   <si>
     <t>Итог:</t>
+  </si>
+  <si>
+    <t>582 941</t>
+  </si>
+  <si>
+    <t>10 000</t>
   </si>
 </sst>
 </file>
@@ -1007,15 +1013,15 @@
       <alignment readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="0"/>
     </xf>
     <xf borderId="1" fillId="2" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFill="1" applyFont="1">
-      <alignment readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="0"/>
+      <alignment shrinkToFit="0" vertical="bottom" wrapText="0"/>
     </xf>
     <xf borderId="0" fillId="0" fontId="2" numFmtId="0" xfId="0" applyFont="1"/>
     <xf borderId="2" fillId="2" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="0"/>
+      <alignment shrinkToFit="0" vertical="bottom" wrapText="0"/>
     </xf>
     <xf borderId="3" fillId="0" fontId="3" numFmtId="0" xfId="0" applyBorder="1" applyFont="1"/>
     <xf borderId="1" fillId="2" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment shrinkToFit="0" vertical="bottom" wrapText="0"/>
+      <alignment readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="0"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1234,6 +1240,7 @@
     <col customWidth="1" min="2" max="2" width="13.67"/>
     <col customWidth="1" min="3" max="3" width="9.33"/>
     <col customWidth="1" min="4" max="4" width="16.78"/>
+    <col customWidth="1" min="5" max="6" width="11.22"/>
   </cols>
   <sheetData>
     <row r="1">
@@ -2355,10 +2362,12 @@
         <v>303</v>
       </c>
       <c r="B102" s="4"/>
-      <c r="C102" s="1">
-        <v>582941.0</v>
-      </c>
-      <c r="D102" s="5"/>
+      <c r="C102" s="1" t="s">
+        <v>304</v>
+      </c>
+      <c r="D102" s="5" t="s">
+        <v>305</v>
+      </c>
     </row>
     <row r="103" ht="15.75" customHeight="1"/>
     <row r="104" ht="15.75" customHeight="1"/>

</xml_diff>